<commit_message>
First report to COLBE done
</commit_message>
<xml_diff>
--- a/data/all-variables.xlsx
+++ b/data/all-variables.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikewood/Dropbox/COLBE/Overheating-analysis-work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikewood/Dropbox/COLBE/Git-cntl-weather-file-analysis/Weather file analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>p1</t>
   </si>
@@ -258,6 +258,30 @@
   </si>
   <si>
     <t>Vary?</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Number of internal paritions</t>
+  </si>
+  <si>
+    <t>Heat in Watts</t>
+  </si>
+  <si>
+    <t>Litres per person per sec?</t>
+  </si>
+  <si>
+    <t>Types (options 1, 2, 3?)</t>
+  </si>
+  <si>
+    <t>Thermal mass of external walls</t>
+  </si>
+  <si>
+    <t>Roof</t>
+  </si>
+  <si>
+    <t>Alfonso (type of building)</t>
   </si>
 </sst>
 </file>
@@ -624,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +659,7 @@
     <col min="2" max="2" width="51.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -651,8 +675,11 @@
       <c r="E1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -668,8 +695,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -686,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -703,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -720,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -737,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -754,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -771,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -788,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -805,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -822,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -839,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -856,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -873,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -890,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -906,8 +936,11 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -924,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -940,8 +973,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -958,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -975,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -992,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1026,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1042,8 +1078,11 @@
       <c r="E24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1060,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1077,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1094,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1111,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1128,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1145,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1161,8 +1200,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1178,8 +1220,11 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1195,8 +1240,11 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1213,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1230,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1247,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>

</xml_diff>